<commit_message>
last version of code before handing in thesis
</commit_message>
<xml_diff>
--- a/logs/switching_showcase.xlsx
+++ b/logs/switching_showcase.xlsx
@@ -104,12 +104,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -124,9 +130,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -165,10 +172,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.13172298070338873"/>
-          <c:y val="5.1014483439099222E-2"/>
-          <c:w val="0.82927769127657991"/>
-          <c:h val="0.81042909587031697"/>
+          <c:x val="6.2757456118728461E-2"/>
+          <c:y val="0.1323914740756221"/>
+          <c:w val="0.89824321586124012"/>
+          <c:h val="0.72905190396012665"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -3211,17 +3218,7 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout>
-        <c:manualLayout>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0"/>
-          <c:y val="0.26369167557166123"/>
-          <c:w val="0.12664687532508934"/>
-          <c:h val="0.42253837691194507"/>
-        </c:manualLayout>
-      </c:layout>
+      <c:legendPos val="t"/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3310,10 +3307,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.13188525252594083"/>
-          <c:y val="6.035665294924554E-2"/>
-          <c:w val="0.82691101424254676"/>
-          <c:h val="0.81235518399706208"/>
+          <c:x val="6.1567462753346083E-2"/>
+          <c:y val="0.12620027434842249"/>
+          <c:w val="0.89722880401514149"/>
+          <c:h val="0.74651156259788509"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -5574,8 +5571,8 @@
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -5640,8 +5637,8 @@
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -5665,17 +5662,7 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout>
-        <c:manualLayout>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0"/>
-          <c:y val="0.39643260641802491"/>
-          <c:w val="9.0696639109915628E-2"/>
-          <c:h val="0.18518648131946469"/>
-        </c:manualLayout>
-      </c:layout>
+      <c:legendPos val="t"/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5692,8 +5679,8 @@
             <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
@@ -5729,7 +5716,14 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr/>
+        <a:defRPr>
+          <a:solidFill>
+            <a:schemeClr val="tx1">
+              <a:lumMod val="50000"/>
+              <a:lumOff val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:defRPr>
       </a:pPr>
       <a:endParaRPr lang="de-DE"/>
     </a:p>
@@ -9231,12 +9225,12 @@
 <c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.0573</cdr:x>
-      <cdr:y>0.04617</cdr:y>
+      <cdr:x>0</cdr:x>
+      <cdr:y>0.13537</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.13337</cdr:x>
-      <cdr:y>0.17371</cdr:y>
+      <cdr:x>0.07099</cdr:x>
+      <cdr:y>0.26291</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
@@ -9251,8 +9245,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="538162" y="93662"/>
-          <a:ext cx="714375" cy="258762"/>
+          <a:off x="0" y="274645"/>
+          <a:ext cx="666749" cy="258756"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -9328,22 +9322,36 @@
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:pPr algn="r"/>
           <a:r>
-            <a:rPr lang="de-DE" sz="1000"/>
+            <a:rPr lang="de-DE" sz="900">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
             <a:t>DISCHARGE</a:t>
           </a:r>
-          <a:endParaRPr lang="de-DE" sz="1100"/>
+          <a:endParaRPr lang="de-DE" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="65000"/>
+                <a:lumOff val="35000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:endParaRPr>
         </a:p>
       </cdr:txBody>
     </cdr:sp>
   </cdr:relSizeAnchor>
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.08857</cdr:x>
-      <cdr:y>0.72222</cdr:y>
+      <cdr:x>0.02721</cdr:x>
+      <cdr:y>0.74335</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.13083</cdr:x>
-      <cdr:y>0.84977</cdr:y>
+      <cdr:x>0.06947</cdr:x>
+      <cdr:y>0.8709</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
@@ -9358,8 +9366,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="831850" y="1465262"/>
-          <a:ext cx="396874" cy="258762"/>
+          <a:off x="255556" y="1508120"/>
+          <a:ext cx="396891" cy="258777"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -9435,22 +9443,36 @@
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:pPr algn="r"/>
           <a:r>
-            <a:rPr lang="de-DE" sz="1000"/>
+            <a:rPr lang="de-DE" sz="900">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
             <a:t>IDLE</a:t>
           </a:r>
-          <a:endParaRPr lang="de-DE" sz="1100"/>
+          <a:endParaRPr lang="de-DE" sz="1050">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="65000"/>
+                <a:lumOff val="35000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:endParaRPr>
         </a:p>
       </cdr:txBody>
     </cdr:sp>
   </cdr:relSizeAnchor>
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.50786</cdr:x>
-      <cdr:y>0.87246</cdr:y>
+      <cdr:x>0.46222</cdr:x>
+      <cdr:y>0.85603</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.61756</cdr:x>
-      <cdr:y>1</cdr:y>
+      <cdr:x>0.57192</cdr:x>
+      <cdr:y>0.98357</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
@@ -9465,8 +9487,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="4769609" y="1783070"/>
-          <a:ext cx="1030287" cy="260663"/>
+          <a:off x="4341018" y="1736731"/>
+          <a:ext cx="1030264" cy="258756"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -9541,8 +9563,15 @@
         </a:lstStyle>
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:r>
-            <a:rPr lang="de-DE" sz="1000"/>
-            <a:t>time in s</a:t>
+            <a:rPr lang="de-DE" sz="900">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Time in seconds</a:t>
           </a:r>
         </a:p>
       </cdr:txBody>
@@ -9555,12 +9584,12 @@
 <c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.50541</cdr:x>
-      <cdr:y>0.8882</cdr:y>
+      <cdr:x>0.46383</cdr:x>
+      <cdr:y>0.88203</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.61511</cdr:x>
-      <cdr:y>1</cdr:y>
+      <cdr:x>0.57353</cdr:x>
+      <cdr:y>0.99383</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
@@ -9575,8 +9604,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="4746625" y="2055813"/>
-          <a:ext cx="1030287" cy="258762"/>
+          <a:off x="4356104" y="2041518"/>
+          <a:ext cx="1030264" cy="258769"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -9651,8 +9680,15 @@
         </a:lstStyle>
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:r>
-            <a:rPr lang="de-DE" sz="1000"/>
-            <a:t>time in s</a:t>
+            <a:rPr lang="de-DE" sz="900">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Time in seconds</a:t>
           </a:r>
         </a:p>
       </cdr:txBody>
@@ -9660,12 +9696,12 @@
   </cdr:relSizeAnchor>
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.0262</cdr:x>
-      <cdr:y>0.00549</cdr:y>
+      <cdr:x>0.00254</cdr:x>
+      <cdr:y>0.00961</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.10091</cdr:x>
-      <cdr:y>0.21605</cdr:y>
+      <cdr:x>0.08519</cdr:x>
+      <cdr:y>0.22017</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
@@ -9680,8 +9716,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="246062" y="12700"/>
-          <a:ext cx="701676" cy="487362"/>
+          <a:off x="23812" y="22232"/>
+          <a:ext cx="776259" cy="487357"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -9757,15 +9793,15 @@
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:pPr algn="r"/>
           <a:r>
-            <a:rPr lang="de-DE" sz="1000"/>
-            <a:t>current</a:t>
-          </a:r>
-          <a:br>
-            <a:rPr lang="de-DE" sz="1000"/>
-          </a:br>
-          <a:r>
-            <a:rPr lang="de-DE" sz="1000"/>
-            <a:t>in mA</a:t>
+            <a:rPr lang="de-DE" sz="900">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Current in mA</a:t>
           </a:r>
         </a:p>
       </cdr:txBody>
@@ -17318,17 +17354,434 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:N26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N29" sqref="N29"/>
+      <selection activeCell="N21" sqref="N21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="16384" width="10.6640625" style="1"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A1" s="2"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+      <c r="N15" s="2"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+      <c r="N16" s="2"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
+      <c r="M17" s="2"/>
+      <c r="N17" s="2"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
+      <c r="N18" s="2"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A19" s="2"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="2"/>
+      <c r="M19" s="2"/>
+      <c r="N19" s="2"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2"/>
+      <c r="L20" s="2"/>
+      <c r="M20" s="2"/>
+      <c r="N20" s="2"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
+      <c r="K21" s="2"/>
+      <c r="L21" s="2"/>
+      <c r="M21" s="2"/>
+      <c r="N21" s="2"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A22" s="2"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="2"/>
+      <c r="L22" s="2"/>
+      <c r="M22" s="2"/>
+      <c r="N22" s="2"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A23" s="2"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="2"/>
+      <c r="L23" s="2"/>
+      <c r="M23" s="2"/>
+      <c r="N23" s="2"/>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A24" s="2"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
+      <c r="L24" s="2"/>
+      <c r="M24" s="2"/>
+      <c r="N24" s="2"/>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A25" s="2"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="2"/>
+      <c r="L25" s="2"/>
+      <c r="M25" s="2"/>
+      <c r="N25" s="2"/>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A26" s="2"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="2"/>
+      <c r="L26" s="2"/>
+      <c r="M26" s="2"/>
+      <c r="N26" s="2"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>